<commit_message>
Deploying to gh-pages from  @ 3dd8f6e7cc9dc62f9510586abb98dc19844888b1 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_6-1-1.xlsx
+++ b/assets/excel/2021_6-1-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77B24779-C3F1-4352-B60C-36DCE94ABC01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8F2FF5-3AC9-4C6E-9F05-F40C369D0479}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{3BD916D0-96AA-4162-A3E2-566C9670FBDD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11208" xr2:uid="{3BD916D0-96AA-4162-A3E2-566C9670FBDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
@@ -125,6 +125,9 @@
       </rPr>
       <t xml:space="preserve"> in Niedersachsen und Deutschland nach Zuwanderungsgeschichte und Nationalität</t>
     </r>
+  </si>
+  <si>
+    <t>3) Die Ergebnisse des Mikrozensus 2020 sind unter anderem aufgrund methodischer Effekte im Rahmen einer Neugestaltung der Erhebung sowie insbesondere aufgrund der Folgen der Corona-Pandemie in Ihrer Datenqualität eingeschränkt. Auf die Verwendung dieser Ergebnisse wird daher verzichtet. Weitere Informationen zur methodischen Neugestaltung des Mikrozensus ab 2020 und zu den Auswirkungen der Neugestaltung und der Corona-Krise auf die Ergebnisse des Jahres 2020 finden Sie auf der Informationsseite des Statistischen Bundesamtes</t>
   </si>
 </sst>
 </file>
@@ -324,46 +327,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -393,27 +366,57 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -809,58 +812,58 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D21238-0549-42DB-A6FD-8D520D9B7866}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="B1:O29"/>
+  <dimension ref="B1:O30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="4" max="14" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="4" max="14" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+    <row r="2" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-    </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="35" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+    </row>
+    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
@@ -872,752 +875,769 @@
       <c r="J5" s="2"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-    </row>
-    <row r="7" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10">
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+    </row>
+    <row r="7" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="27"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="4">
         <v>2005</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="5">
         <v>2007</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="5">
         <v>2009</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="6">
         <v>2010</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="5">
         <v>2012</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="6">
         <v>2013</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="6">
         <v>2014</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="6">
         <v>2015</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="6">
         <v>2016</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="6">
         <v>2017</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="7">
         <v>2018</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="7">
         <v>2019</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
+    <row r="8" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="28"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-    </row>
-    <row r="9" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="18">
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+    </row>
+    <row r="9" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="8">
         <v>1</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="8">
         <v>2</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="8">
         <v>3</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="8">
         <v>4</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="8">
         <v>5</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="8">
         <v>6</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="8">
         <v>7</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="8">
         <v>8</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="8">
         <v>9</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="8">
         <v>10</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="8">
         <v>11</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="8">
         <v>12</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="9">
         <v>13</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="9">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
+    <row r="10" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="11">
         <v>13.1</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="11">
         <v>12.8</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="11">
         <v>13</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="11">
         <v>12.9</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="11">
         <v>13.9</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="11">
         <v>14.5</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="11">
         <v>13.8</v>
       </c>
-      <c r="K10" s="21">
+      <c r="K10" s="11">
         <v>14</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="11">
         <v>13.5</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="11">
         <v>13.3</v>
       </c>
-      <c r="N10" s="22">
+      <c r="N10" s="12">
         <v>12.5</v>
       </c>
-      <c r="O10" s="22">
+      <c r="O10" s="12">
         <f>'[1]A3.9 NI_Land'!P55</f>
         <v>13.4</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
+    <row r="11" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="11">
         <v>43</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="11">
         <v>40.299999999999997</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="11">
         <v>37.9</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="11">
         <v>36.700000000000003</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="11">
         <v>36.5</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="11">
         <v>36</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="11">
         <v>36.6</v>
       </c>
-      <c r="K11" s="21">
+      <c r="K11" s="11">
         <v>40.5</v>
       </c>
-      <c r="L11" s="21">
+      <c r="L11" s="11">
         <v>43</v>
       </c>
-      <c r="M11" s="21">
+      <c r="M11" s="11">
         <v>41</v>
       </c>
-      <c r="N11" s="22">
+      <c r="N11" s="12">
         <v>38.5</v>
       </c>
-      <c r="O11" s="22">
+      <c r="O11" s="12">
         <f>'[1]A3.9 NI_Land'!P54</f>
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
+    <row r="12" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="11">
         <v>33.200000000000003</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="11">
         <v>32.200000000000003</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="11">
         <v>29.7</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="11">
         <v>29.1</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="11">
         <v>28.7</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="11">
         <v>28.5</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="11">
         <v>27.7</v>
       </c>
-      <c r="K12" s="21">
+      <c r="K12" s="11">
         <v>30.2</v>
       </c>
-      <c r="L12" s="21">
+      <c r="L12" s="11">
         <v>30.9</v>
       </c>
-      <c r="M12" s="21">
+      <c r="M12" s="11">
         <v>30.1</v>
       </c>
-      <c r="N12" s="22">
+      <c r="N12" s="12">
         <v>28.2</v>
       </c>
-      <c r="O12" s="22">
+      <c r="O12" s="12">
         <f>'[1]A3.9 NI_Land'!P57</f>
         <v>30.4</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+    <row r="13" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="11">
         <v>11.7</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="11">
         <v>11.3</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="11">
         <v>11.5</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="11">
         <v>11.5</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="11">
         <v>12.4</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="11">
         <v>13</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="11">
         <v>12.6</v>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="11">
         <v>12.7</v>
       </c>
-      <c r="L13" s="21">
+      <c r="L13" s="11">
         <v>12.2</v>
       </c>
-      <c r="M13" s="21">
+      <c r="M13" s="11">
         <v>11.9</v>
       </c>
-      <c r="N13" s="22">
+      <c r="N13" s="12">
         <v>11.2</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="12">
         <f>'[1]A3.9 NI_Land'!P58</f>
         <v>11.9</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="23" t="s">
+    <row r="14" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="14">
         <v>15.1</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="14">
         <v>14.7</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="14">
         <v>14.6</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="14">
         <v>14.5</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="14">
         <v>15.2</v>
       </c>
-      <c r="I14" s="24">
+      <c r="I14" s="14">
         <v>15.8</v>
       </c>
-      <c r="J14" s="24">
+      <c r="J14" s="14">
         <v>15.3</v>
       </c>
-      <c r="K14" s="24">
+      <c r="K14" s="14">
         <v>15.9</v>
       </c>
-      <c r="L14" s="24">
+      <c r="L14" s="14">
         <v>16</v>
       </c>
-      <c r="M14" s="24">
+      <c r="M14" s="14">
         <v>15.8</v>
       </c>
-      <c r="N14" s="25">
+      <c r="N14" s="15">
         <v>15</v>
       </c>
-      <c r="O14" s="25">
+      <c r="O14" s="15">
         <f>'[1]A3.9 NI_Land'!P6</f>
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
+    <row r="15" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="11">
         <v>12.8</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="11">
         <v>12.5</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="11">
         <v>13</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="11">
         <v>12.9</v>
       </c>
-      <c r="H15" s="21">
+      <c r="H15" s="11">
         <v>13.6</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="11">
         <v>13.9</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J15" s="11">
         <v>13.7</v>
       </c>
-      <c r="K15" s="21">
+      <c r="K15" s="11">
         <v>13.8</v>
       </c>
-      <c r="L15" s="21">
+      <c r="L15" s="11">
         <v>13.3</v>
       </c>
-      <c r="M15" s="21">
+      <c r="M15" s="11">
         <v>13.1</v>
       </c>
-      <c r="N15" s="22">
+      <c r="N15" s="12">
         <v>12.8</v>
       </c>
-      <c r="O15" s="22">
+      <c r="O15" s="12">
         <f>'[1]A2.0 DE_Bund'!P55</f>
         <v>13.2</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
+    <row r="16" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="11">
         <v>34.299999999999997</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="11">
         <v>32.6</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="11">
         <v>31.8</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="11">
         <v>31.7</v>
       </c>
-      <c r="H16" s="21">
+      <c r="H16" s="11">
         <v>31.5</v>
       </c>
-      <c r="I16" s="21">
+      <c r="I16" s="11">
         <v>32</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="11">
         <v>32.5</v>
       </c>
-      <c r="K16" s="21">
+      <c r="K16" s="11">
         <v>33.700000000000003</v>
       </c>
-      <c r="L16" s="21">
+      <c r="L16" s="11">
         <v>35.5</v>
       </c>
-      <c r="M16" s="21">
+      <c r="M16" s="11">
         <v>36.200000000000003</v>
       </c>
-      <c r="N16" s="22">
+      <c r="N16" s="12">
         <v>34.799999999999997</v>
       </c>
-      <c r="O16" s="22">
+      <c r="O16" s="12">
         <f>'[1]A2.0 DE_Bund'!P54</f>
         <v>35.200000000000003</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
+    <row r="17" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="11">
         <v>28.2</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="11">
         <v>26.9</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="11">
         <v>26.6</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="11">
         <v>26.2</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="11">
         <v>26.3</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="11">
         <v>26.6</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J17" s="11">
         <v>26.7</v>
       </c>
-      <c r="K17" s="21">
+      <c r="K17" s="11">
         <v>27.7</v>
       </c>
-      <c r="L17" s="21">
+      <c r="L17" s="11">
         <v>28</v>
       </c>
-      <c r="M17" s="21">
+      <c r="M17" s="11">
         <v>28.6</v>
       </c>
-      <c r="N17" s="22">
+      <c r="N17" s="12">
         <v>27.2</v>
       </c>
-      <c r="O17" s="22">
+      <c r="O17" s="12">
         <f>'[1]A2.0 DE_Bund'!P57</f>
         <v>27.8</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
+    <row r="18" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="11">
         <v>11.6</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="11">
         <v>11.3</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="11">
         <v>11.7</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="11">
         <v>11.7</v>
       </c>
-      <c r="H18" s="21">
+      <c r="H18" s="11">
         <v>12.3</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="11">
         <v>12.6</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="11">
         <v>12.5</v>
       </c>
-      <c r="K18" s="21">
+      <c r="K18" s="11">
         <v>12.5</v>
       </c>
-      <c r="L18" s="21">
+      <c r="L18" s="11">
         <v>12.1</v>
       </c>
-      <c r="M18" s="21">
+      <c r="M18" s="11">
         <v>11.8</v>
       </c>
-      <c r="N18" s="22">
+      <c r="N18" s="12">
         <v>11.4</v>
       </c>
-      <c r="O18" s="22">
+      <c r="O18" s="12">
         <f>'[1]A2.0 DE_Bund'!P58</f>
         <v>11.7</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
+    <row r="19" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="14">
         <v>14.7</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="14">
         <v>14.3</v>
       </c>
-      <c r="F19" s="24">
+      <c r="F19" s="14">
         <v>14.6</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="14">
         <v>14.5</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="14">
         <v>15</v>
       </c>
-      <c r="I19" s="24">
+      <c r="I19" s="14">
         <v>15.5</v>
       </c>
-      <c r="J19" s="24">
+      <c r="J19" s="14">
         <v>15.4</v>
       </c>
-      <c r="K19" s="24">
+      <c r="K19" s="14">
         <v>15.7</v>
       </c>
-      <c r="L19" s="24">
+      <c r="L19" s="14">
         <v>15.7</v>
       </c>
-      <c r="M19" s="24">
+      <c r="M19" s="14">
         <v>15.8</v>
       </c>
-      <c r="N19" s="25">
+      <c r="N19" s="15">
         <v>15.5</v>
       </c>
-      <c r="O19" s="25">
+      <c r="O19" s="15">
         <f>'[1]A2.0 DE_Bund'!P6</f>
         <v>15.9</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="26"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-    </row>
-    <row r="21" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="29" t="s">
+    <row r="20" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+    </row>
+    <row r="21" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-    </row>
-    <row r="22" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="30" t="s">
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+    </row>
+    <row r="22" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-    </row>
-    <row r="23" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
-    </row>
-    <row r="24" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="32" t="s">
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+    </row>
+    <row r="23" spans="2:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+    </row>
+    <row r="24" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+    </row>
+    <row r="25" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-    </row>
-    <row r="25" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-    </row>
-    <row r="26" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="32" t="s">
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+    </row>
+    <row r="26" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+    </row>
+    <row r="27" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-    </row>
-    <row r="27" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="32" t="s">
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+    </row>
+    <row r="28" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="32"/>
-    </row>
-    <row r="28" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="32" t="s">
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+    </row>
+    <row r="29" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
-      <c r="M28" s="32"/>
-    </row>
-    <row r="29" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="33" t="s">
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+    </row>
+    <row r="30" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B27:M27"/>
-    <mergeCell ref="B28:M28"/>
-    <mergeCell ref="B29:M29"/>
-    <mergeCell ref="B21:M21"/>
-    <mergeCell ref="B22:M22"/>
-    <mergeCell ref="B23:M23"/>
-    <mergeCell ref="B24:M24"/>
-    <mergeCell ref="B25:M25"/>
-    <mergeCell ref="B26:M26"/>
+  <mergeCells count="14">
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="D6:O6"/>
     <mergeCell ref="D8:O8"/>
+    <mergeCell ref="B23:M23"/>
+    <mergeCell ref="B28:M28"/>
+    <mergeCell ref="B29:M29"/>
+    <mergeCell ref="B30:M30"/>
+    <mergeCell ref="B21:M21"/>
+    <mergeCell ref="B22:M22"/>
+    <mergeCell ref="B24:M24"/>
+    <mergeCell ref="B25:M25"/>
+    <mergeCell ref="B26:M26"/>
+    <mergeCell ref="B27:M27"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B29" r:id="rId1" xr:uid="{66CC8081-BF15-476D-9F54-240770BF8CA1}"/>
+    <hyperlink ref="B30" r:id="rId1" xr:uid="{66CC8081-BF15-476D-9F54-240770BF8CA1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>